<commit_message>
Implement dynamic rendering for sessions and speakers from JSON data
</commit_message>
<xml_diff>
--- a/devfest-armenia-2025 flattened sessions.xlsx
+++ b/devfest-armenia-2025 flattened sessions.xlsx
@@ -5,14 +5,14 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Sessions and speakers" sheetId="1" r:id="rId1"/>
+    <sheet name="Accepted sessions and speakers" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Session Id</t>
   </si>
@@ -29,13 +29,25 @@
     <t>Owner Email</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Date Submitted</t>
-  </si>
-  <si>
-    <t>Owner Notes</t>
+    <t>Owner Informed</t>
+  </si>
+  <si>
+    <t>Owner Confirmed</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Scheduled At</t>
+  </si>
+  <si>
+    <t>Scheduled Duration</t>
+  </si>
+  <si>
+    <t>Live Link</t>
+  </si>
+  <si>
+    <t>Recording Link</t>
   </si>
   <si>
     <t>Speaker Id</t>
@@ -57,6 +69,39 @@
   </si>
   <si>
     <t>Profile Picture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent  Development Kit Deep Dive</t>
+  </si>
+  <si>
+    <t>From Initialization to Ideation to Prompting to Deployment. All of these and the intermediate steps will be covered in the creation of your own Agent application. We all know about AI, but this is much more than that, it is making sure the AI is deployed and available in the most consistent way possible with all the requirements for application development including version control, testing and scaling being covered. You will be given credits to follow along on the workshop.</t>
+  </si>
+  <si>
+    <t>Ankur Roy</t>
+  </si>
+  <si>
+    <t>ankur.roy@onlinepartner.se</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>8ca460b2-bb7b-4e0a-bc41-7a7ddcb2dda3</t>
+  </si>
+  <si>
+    <t>Ankur</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>Solutions Architect at Online Partner AB | Google Developer Expert in Cloud</t>
+  </si>
+  <si>
+    <t>I am a Solutions Architect at Online Partner AB and a Cloud GDE. I have worked on several projects involving Google Cloud services and Google Workspace along with multiple other technology stacks and platforms.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/7b5c-400o400o1-LM8dCULuUeHrEhCsuRY34o.jpg</t>
   </si>
   <si>
     <t>Ordering Coffee with Firebase AI</t>
@@ -80,7 +125,7 @@
     <t>maxkachinkin@gmail.com</t>
   </si>
   <si>
-    <t>Accepted</t>
+    <t>Room 1</t>
   </si>
   <si>
     <t>1f2ba26b-921a-4b3a-ba24-1e8208f935b8</t>
@@ -129,7 +174,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +184,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF0F8E6" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3" tint="0"/>
       </patternFill>
     </fill>
     <fill>
@@ -163,6 +213,7 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2"/>
     <xf numFmtId="0" fontId="1" fillId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="4"/>
     <xf numFmtId="164" fontId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -174,7 +225,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -196,13 +247,13 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -217,58 +268,126 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
+        <v>1062404</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45953.493480324076</v>
+      </c>
+      <c r="G2" s="4">
+        <v>45953.501328275459</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
         <v>1060533</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="3">
-        <v>45950.775707372683</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>25</v>
+      <c r="B3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45951.567294988425</v>
+      </c>
+      <c r="G3" s="4">
+        <v>45951.575142476853</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="4">
+        <v>46011.375</v>
+      </c>
+      <c r="J3" s="0">
+        <v>30</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>